<commit_message>
No me sube por comando
</commit_message>
<xml_diff>
--- a/Medidas.xlsx
+++ b/Medidas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6415fbc5eb1d0abc/AITOR/GIT/Hotel-DataScience-MachineLearning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{87BCE315-2F71-404A-8CF5-8855E2423D58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83A2F755-547F-44DF-A2A7-7D514A4D37BD}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{87BCE315-2F71-404A-8CF5-8855E2423D58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6EF01D29-DAAA-4895-BEB9-881D5C0BC8E6}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{DF37E74D-0EEE-4FC6-89FB-CBC951E8B9B4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
   <si>
     <t>REG_LOG</t>
   </si>
@@ -185,12 +185,36 @@
   <si>
     <t>es una métrica que mide el error porcentual promedio entre las predicciones del modelo y los valores reales</t>
   </si>
+  <si>
+    <t>"+"</t>
+  </si>
+  <si>
+    <t>NPB</t>
+  </si>
+  <si>
+    <t>"-"</t>
+  </si>
+  <si>
+    <t>VPN</t>
+  </si>
+  <si>
+    <t>0.8850514105</t>
+  </si>
+  <si>
+    <t>mide la proporción de verdaderos negativos sobre el total de predicciones negativas realizadas por el modelo</t>
+  </si>
+  <si>
+    <t>f1-score Negativo</t>
+  </si>
+  <si>
+    <t>0.8936272160996646</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,6 +243,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Segoe UI"/>
@@ -287,7 +318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -300,6 +331,11 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -614,13 +650,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7DFFED3-3896-4534-BCD6-F7A7F804E405}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C19" sqref="C19"/>
+      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -676,6 +712,9 @@
       <c r="D3" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="E3" t="s">
+        <v>43</v>
+      </c>
       <c r="F3" s="4" t="s">
         <v>33</v>
       </c>
@@ -693,6 +732,9 @@
       <c r="D4" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="E4" t="s">
+        <v>45</v>
+      </c>
       <c r="F4" s="4" t="s">
         <v>35</v>
       </c>
@@ -708,99 +750,140 @@
       <c r="D5" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="E5" t="s">
+        <v>43</v>
+      </c>
       <c r="F5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16.5">
       <c r="A6" s="7" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="B6" s="3"/>
-      <c r="C6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>27</v>
+      <c r="C6" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" t="s">
+        <v>45</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16.5">
       <c r="A7" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7" s="3"/>
-      <c r="C7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="3"/>
+      <c r="C7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
+        <v>43</v>
+      </c>
       <c r="F7" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16.5">
       <c r="A8" s="7" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="B8" s="3"/>
-      <c r="C8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="F8" s="4" t="s">
-        <v>39</v>
-      </c>
+      <c r="C8" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="10"/>
     </row>
     <row r="9" spans="1:6" ht="16.5">
       <c r="A9" s="7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="2" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="D9" s="3"/>
       <c r="F9" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16.5">
       <c r="A10" s="7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D10" s="3"/>
       <c r="F10" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16.5">
       <c r="A11" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D11" s="3"/>
       <c r="F11" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16.5">
       <c r="A12" s="7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="F12" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16.5">
+      <c r="A13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="F13" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="3"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="8" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>